<commit_message>
general updates + P_Summaries T_Previews
</commit_message>
<xml_diff>
--- a/User stories.xlsx
+++ b/User stories.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isadora/Documents/CodingNomads/AllProjects/JustDOit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEC59F9-74D0-3A4E-96FB-8650D1CDB29F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707BEFD7-C9FD-F04D-9443-A1371F40493A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{639CDEA4-6362-564C-8B92-F60BAF9910A7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{639CDEA4-6362-564C-8B92-F60BAF9910A7}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
     <sheet name="User stories" sheetId="1" r:id="rId2"/>
     <sheet name="Tables" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Prototype_v1" sheetId="5" r:id="rId4"/>
+    <sheet name="Questions" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'User stories'!$A$1:$E$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'User stories'!$A$1:$E$89</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="224">
   <si>
     <t>Login</t>
   </si>
@@ -240,9 +241,6 @@
     <t>UserRole</t>
   </si>
   <si>
-    <t>UserTask</t>
-  </si>
-  <si>
     <t>Coming Soon!</t>
   </si>
   <si>
@@ -289,9 +287,6 @@
   </si>
   <si>
     <t>roleId</t>
-  </si>
-  <si>
-    <t>role</t>
   </si>
   <si>
     <t>userId</t>
@@ -791,22 +786,49 @@
     <t>taskCreatorUserId</t>
   </si>
   <si>
-    <t>taskProject</t>
-  </si>
-  <si>
     <t>Questions</t>
   </si>
   <si>
     <t xml:space="preserve">on mysql, what is `user`@`%` (instead of @‘localhost’) </t>
   </si>
   <si>
-    <t>how do I join a third table in the POJO?</t>
-  </si>
-  <si>
-    <t>presumably if I wanted emojis in my task description</t>
-  </si>
-  <si>
     <t>&lt;&lt;emojis</t>
+  </si>
+  <si>
+    <t>is a TaskCreator role required? Initial logic for No: all project stakeholders get notified of task activities (whether they created the task or not)</t>
+  </si>
+  <si>
+    <t>save role id when saving stakeholder?</t>
+  </si>
+  <si>
+    <t>taskAddedNotificationOn (Y/N)</t>
+  </si>
+  <si>
+    <t>Household</t>
+  </si>
+  <si>
+    <t>HouseId</t>
+  </si>
+  <si>
+    <t>HouseName</t>
+  </si>
+  <si>
+    <t>HouseMember</t>
+  </si>
+  <si>
+    <t>is it convention for joint tables to be lower case, e.g. userrole instead of userRole</t>
+  </si>
+  <si>
+    <t>roleName</t>
+  </si>
+  <si>
+    <t>arrange by</t>
+  </si>
+  <si>
+    <t>Prority??</t>
+  </si>
+  <si>
+    <t>MainProjectId</t>
   </si>
 </sst>
 </file>
@@ -816,7 +838,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -961,6 +983,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="21">
     <fill>
@@ -1055,12 +1091,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB3B4FC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1080,6 +1110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF787B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1120,7 +1156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1236,16 +1272,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1272,8 +1305,8 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1311,9 +1344,6 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1341,19 +1371,19 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -1365,6 +1395,18 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1401,68 +1443,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39CB4464-DA16-754F-BC07-E593F5F90608}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1168400" y="800100"/>
-          <a:ext cx="2781300" cy="2057400"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1478,60 +1467,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1308100" y="800100"/>
-          <a:ext cx="1917700" cy="2451100"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{249DA024-6E97-9746-AD25-4ACDE24F91F9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5753100" y="1219200"/>
-          <a:ext cx="12700" cy="2057400"/>
+          <a:ext cx="1879600" cy="2679700"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1567,7 +1503,7 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1620,7 +1556,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1666,15 +1602,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
+      <xdr:colOff>596900</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1689,114 +1625,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3213100" y="482600"/>
-          <a:ext cx="1968500" cy="2768600"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37107346-B3B1-CB4B-8E0B-7F692D50C3B8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3924300" y="673100"/>
-          <a:ext cx="2933700" cy="2184400"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="39" name="Straight Arrow Connector 38">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA62815C-349D-B04D-AD41-FE03D6EFB3EF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5130800" y="673100"/>
-          <a:ext cx="1727200" cy="1981200"/>
+          <a:off x="3187700" y="482600"/>
+          <a:ext cx="1993900" cy="2997200"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1825,15 +1655,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
+      <xdr:colOff>596900</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1848,8 +1678,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3213100" y="622300"/>
-          <a:ext cx="12700" cy="2628900"/>
+          <a:off x="3187700" y="622300"/>
+          <a:ext cx="38100" cy="2857500"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1879,13 +1709,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1066800</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>292100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1939,13 +1769,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>977900</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>292100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1999,13 +1829,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>977900</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2059,13 +1889,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1016000</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2119,13 +1949,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1003300</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>279400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2179,13 +2009,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1079500</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>330200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2239,13 +2069,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>330200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2299,13 +2129,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2359,13 +2189,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2419,13 +2249,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1016000</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>317500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2473,6 +2303,167 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C781601E-E6BF-9B42-A440-3D8AD0ACA40F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1308100" y="800100"/>
+          <a:ext cx="4508500" cy="2463800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADC75F4A-FBCD-F142-89B5-036655EE2037}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5753100" y="406400"/>
+          <a:ext cx="5575300" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>347816</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A175C782-72A3-794C-B94E-D549C44AF3BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="177800"/>
+          <a:ext cx="9987116" cy="7772400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2775,86 +2766,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB8ADFF-DB37-574A-B3A7-73C2E57BCC69}">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:A35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="225" style="92" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="91"/>
+    <col min="1" max="1" width="225" style="89" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="88"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="90" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17">
+      <c r="A2" s="89" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="34">
+      <c r="A3" s="89" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="17">
+      <c r="A5" s="87" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="34">
+      <c r="A6" s="89" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="17">
+      <c r="A8" s="87" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="17">
+      <c r="A9" s="89" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="17">
+      <c r="A10" s="89" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="17">
+      <c r="A13" s="90" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="17">
+      <c r="A21" s="90" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="68">
+      <c r="A22" s="89" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="17">
+      <c r="A23" s="89" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="17">
+      <c r="A24" s="89" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="17">
+      <c r="A29" s="90" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17">
-      <c r="A2" s="92" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="34">
-      <c r="A3" s="92" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="17">
-      <c r="A5" s="90" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="34">
-      <c r="A6" s="92" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="17">
-      <c r="A8" s="90" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="17">
-      <c r="A9" s="92" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="17">
-      <c r="A10" s="92" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="17">
-      <c r="A13" s="93" t="s">
+    <row r="35" spans="1:1" ht="17">
+      <c r="A35" s="90" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="17">
-      <c r="A21" s="93" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="68">
-      <c r="A22" s="92" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="17">
-      <c r="A23" s="92" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="17">
-      <c r="A25" s="93" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="17">
-      <c r="A31" s="93" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2864,10 +2860,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1D78FB-BE4E-CB42-B499-DD12355D68EB}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1"/>
@@ -2882,7 +2879,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19">
       <c r="A1" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>3</v>
@@ -2900,12 +2897,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" hidden="1">
       <c r="A2" s="31">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="9">
         <v>3</v>
@@ -2920,13 +2917,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" hidden="1">
       <c r="A3" s="31">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="9">
         <f>C2</f>
@@ -2942,182 +2939,182 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="67">
+    <row r="4" spans="1:6" hidden="1">
+      <c r="A4" s="64">
         <f t="shared" ref="A4:A9" si="0">A3+0.1</f>
         <v>2.1</v>
       </c>
-      <c r="B4" s="68" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="66">
+      <c r="B4" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="63">
         <f>C2</f>
         <v>3</v>
       </c>
-      <c r="D4" s="65" t="str">
+      <c r="D4" s="62" t="str">
         <f>D2</f>
         <v>Login</v>
       </c>
-      <c r="E4" s="65" t="str">
+      <c r="E4" s="62" t="str">
         <f>E2</f>
         <v>Login</v>
       </c>
-      <c r="F4" s="65" t="str">
+      <c r="F4" s="62" t="str">
         <f>F2</f>
         <v>L</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="67">
+    <row r="5" spans="1:6" hidden="1">
+      <c r="A5" s="64">
         <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="B5" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="66">
-        <f>C2</f>
+      <c r="B5" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="63">
+        <f t="shared" ref="C5:F7" si="1">C2</f>
         <v>3</v>
       </c>
-      <c r="D5" s="65" t="str">
-        <f>D2</f>
+      <c r="D5" s="62" t="str">
+        <f t="shared" si="1"/>
         <v>Login</v>
       </c>
-      <c r="E5" s="65" t="str">
-        <f>E2</f>
+      <c r="E5" s="62" t="str">
+        <f t="shared" si="1"/>
         <v>Login</v>
       </c>
-      <c r="F5" s="65" t="str">
-        <f>F2</f>
+      <c r="F5" s="62" t="str">
+        <f t="shared" si="1"/>
         <v>L</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="67">
+    <row r="6" spans="1:6" hidden="1">
+      <c r="A6" s="64">
         <f t="shared" si="0"/>
         <v>2.3000000000000003</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" s="66">
-        <f>C3</f>
+      <c r="B6" s="65" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="63">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D6" s="65" t="str">
-        <f>D3</f>
+      <c r="D6" s="62" t="str">
+        <f t="shared" si="1"/>
         <v>Login</v>
       </c>
-      <c r="E6" s="65" t="str">
-        <f>E3</f>
+      <c r="E6" s="62" t="str">
+        <f t="shared" si="1"/>
         <v>Login</v>
       </c>
-      <c r="F6" s="65" t="str">
-        <f>F3</f>
+      <c r="F6" s="62" t="str">
+        <f t="shared" si="1"/>
         <v>L</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="67">
-        <f t="shared" ref="A7" si="1">A6+0.1</f>
+    <row r="7" spans="1:6" hidden="1">
+      <c r="A7" s="64">
+        <f t="shared" ref="A7" si="2">A6+0.1</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="B7" s="68" t="s">
-        <v>183</v>
-      </c>
-      <c r="C7" s="66">
+      <c r="B7" s="65" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="63">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D7" s="62" t="str">
+        <f t="shared" si="1"/>
+        <v>Login</v>
+      </c>
+      <c r="E7" s="62" t="str">
+        <f t="shared" si="1"/>
+        <v>Login</v>
+      </c>
+      <c r="F7" s="62" t="str">
+        <f t="shared" si="1"/>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1">
+      <c r="A8" s="64">
+        <f>A6+0.1</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" s="63">
         <f>C4</f>
         <v>3</v>
       </c>
-      <c r="D7" s="65" t="str">
+      <c r="D8" s="62" t="str">
         <f>D4</f>
         <v>Login</v>
       </c>
-      <c r="E7" s="65" t="str">
+      <c r="E8" s="62" t="str">
         <f>E4</f>
         <v>Login</v>
       </c>
-      <c r="F7" s="65" t="str">
+      <c r="F8" s="62" t="str">
         <f>F4</f>
         <v>L</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="67">
-        <f>A6+0.1</f>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="B8" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="C8" s="66">
-        <f>C4</f>
-        <v>3</v>
-      </c>
-      <c r="D8" s="65" t="str">
-        <f>D4</f>
-        <v>Login</v>
-      </c>
-      <c r="E8" s="65" t="str">
-        <f>E4</f>
-        <v>Login</v>
-      </c>
-      <c r="F8" s="65" t="str">
-        <f>F4</f>
-        <v>L</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="67">
+    <row r="9" spans="1:6" hidden="1">
+      <c r="A9" s="64">
         <f t="shared" si="0"/>
         <v>2.5000000000000004</v>
       </c>
-      <c r="B9" s="68" t="s">
-        <v>184</v>
-      </c>
-      <c r="C9" s="66">
+      <c r="B9" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" s="63">
         <f>C6</f>
         <v>3</v>
       </c>
-      <c r="D9" s="65" t="str">
+      <c r="D9" s="62" t="str">
         <f>D6</f>
         <v>Login</v>
       </c>
-      <c r="E9" s="65" t="str">
+      <c r="E9" s="62" t="str">
         <f>E6</f>
         <v>Login</v>
       </c>
-      <c r="F9" s="65" t="str">
+      <c r="F9" s="62" t="str">
         <f>F6</f>
         <v>L</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="67">
-        <f t="shared" ref="A10" si="2">A9+0.1</f>
+    <row r="10" spans="1:6" hidden="1">
+      <c r="A10" s="64">
+        <f t="shared" ref="A10" si="3">A9+0.1</f>
         <v>2.6000000000000005</v>
       </c>
-      <c r="B10" s="68" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="66">
+      <c r="B10" s="65" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="63">
         <f>C9</f>
         <v>3</v>
       </c>
-      <c r="D10" s="65" t="str">
-        <f t="shared" ref="D10:E10" si="3">D9</f>
+      <c r="D10" s="62" t="str">
+        <f t="shared" ref="D10:E10" si="4">D9</f>
         <v>Login</v>
       </c>
-      <c r="E10" s="65" t="str">
-        <f t="shared" si="3"/>
+      <c r="E10" s="62" t="str">
+        <f t="shared" si="4"/>
         <v>Login</v>
       </c>
-      <c r="F10" s="65" t="str">
+      <c r="F10" s="62" t="str">
         <f>F9</f>
         <v>L</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" hidden="1">
       <c r="A11" s="31">
         <f>A3+1</f>
         <v>3</v>
@@ -3139,16 +3136,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" hidden="1">
       <c r="A12" s="31">
-        <f t="shared" ref="A12:A85" si="4">A11+1</f>
+        <f t="shared" ref="A12:A85" si="5">A11+1</f>
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C12" s="9">
-        <f t="shared" ref="C12:C13" si="5">C11</f>
+        <f t="shared" ref="C12:C13" si="6">C11</f>
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -3161,16 +3158,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" hidden="1">
       <c r="A13" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -3183,32 +3180,32 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="67">
+    <row r="14" spans="1:6" hidden="1">
+      <c r="A14" s="64">
         <f>A13+0.1</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="B14" s="68" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="66">
+      <c r="B14" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="63">
         <f>C13</f>
         <v>3</v>
       </c>
-      <c r="D14" s="65" t="str">
-        <f t="shared" ref="D14" si="6">D13</f>
+      <c r="D14" s="62" t="str">
+        <f t="shared" ref="D14" si="7">D13</f>
         <v>Login</v>
       </c>
-      <c r="E14" s="65" t="str">
-        <f t="shared" ref="E14" si="7">E13</f>
+      <c r="E14" s="62" t="str">
+        <f t="shared" ref="E14" si="8">E13</f>
         <v>Login</v>
       </c>
-      <c r="F14" s="65" t="str">
+      <c r="F14" s="62" t="str">
         <f>F13</f>
         <v>L</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" hidden="1">
       <c r="A15" s="32">
         <f>A13+1</f>
         <v>6</v>
@@ -3229,13 +3226,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="74" customFormat="1">
+    <row r="16" spans="1:6" s="71" customFormat="1" hidden="1">
       <c r="A16" s="32">
         <f>A15+1</f>
         <v>7</v>
       </c>
-      <c r="B16" s="73" t="s">
-        <v>74</v>
+      <c r="B16" s="70" t="s">
+        <v>73</v>
       </c>
       <c r="C16" s="10">
         <f>C15</f>
@@ -3251,57 +3248,57 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="72" customFormat="1">
-      <c r="A17" s="69">
+    <row r="17" spans="1:7" s="69" customFormat="1" hidden="1">
+      <c r="A17" s="66">
         <f>A16+0.1</f>
         <v>7.1</v>
       </c>
-      <c r="B17" s="75" t="s">
-        <v>204</v>
-      </c>
-      <c r="C17" s="71">
+      <c r="B17" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="C17" s="68">
         <f>C16</f>
         <v>3</v>
       </c>
-      <c r="D17" s="70" t="str">
-        <f t="shared" ref="D17:D18" si="8">D16</f>
+      <c r="D17" s="67" t="str">
+        <f t="shared" ref="D17:D18" si="9">D16</f>
         <v>Registration</v>
       </c>
-      <c r="E17" s="70" t="str">
-        <f t="shared" ref="E17:E18" si="9">E16</f>
+      <c r="E17" s="67" t="str">
+        <f t="shared" ref="E17:E18" si="10">E16</f>
         <v>Registration</v>
       </c>
-      <c r="F17" s="70" t="str">
-        <f t="shared" ref="F17:F18" si="10">F16</f>
+      <c r="F17" s="67" t="str">
+        <f t="shared" ref="F17:F18" si="11">F16</f>
         <v>L</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="72" customFormat="1">
-      <c r="A18" s="69">
-        <f t="shared" si="4"/>
+    <row r="18" spans="1:7" s="69" customFormat="1" hidden="1">
+      <c r="A18" s="66">
+        <f t="shared" si="5"/>
         <v>8.1</v>
       </c>
-      <c r="B18" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="C18" s="71">
-        <f t="shared" ref="C18" si="11">C17</f>
+      <c r="B18" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="68">
+        <f t="shared" ref="C18" si="12">C17</f>
         <v>3</v>
       </c>
-      <c r="D18" s="70" t="str">
-        <f t="shared" si="8"/>
-        <v>Registration</v>
-      </c>
-      <c r="E18" s="70" t="str">
+      <c r="D18" s="67" t="str">
         <f t="shared" si="9"/>
         <v>Registration</v>
       </c>
-      <c r="F18" s="70" t="str">
+      <c r="E18" s="67" t="str">
         <f t="shared" si="10"/>
+        <v>Registration</v>
+      </c>
+      <c r="F18" s="67" t="str">
+        <f t="shared" si="11"/>
         <v>L</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" hidden="1">
       <c r="A19" s="32">
         <f>A16+1</f>
         <v>8</v>
@@ -3322,9 +3319,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" hidden="1">
       <c r="A20" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -3345,7 +3342,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="B21" s="18" t="s">
@@ -3364,7 +3361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" s="33">
         <f>A21+1</f>
         <v>11</v>
@@ -3385,9 +3382,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="B23" s="18" t="s">
@@ -3406,7 +3403,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" hidden="1">
       <c r="A24" s="33">
         <f>A23+1</f>
         <v>13</v>
@@ -3430,13 +3427,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" hidden="1">
       <c r="A25" s="33">
         <f>A24+1</f>
         <v>14</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C25" s="19">
         <v>4</v>
@@ -3452,9 +3449,9 @@
       </c>
       <c r="G25" s="28"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" hidden="1">
       <c r="A26" s="33">
-        <f t="shared" ref="A26:A28" si="12">A25+1</f>
+        <f t="shared" ref="A26:A28" si="13">A25+1</f>
         <v>15</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3473,13 +3470,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>16</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C27" s="19">
         <v>5</v>
@@ -3494,13 +3491,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C28" s="19">
         <v>5</v>
@@ -3509,19 +3506,19 @@
         <v>26</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="F28" s="110" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" s="106" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="33">
-        <f t="shared" ref="A29" si="13">A28+1</f>
+        <f t="shared" ref="A29" si="14">A28+1</f>
         <v>18</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C29" s="19">
         <v>5</v>
@@ -3530,13 +3527,13 @@
         <v>26</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="F29" s="110" t="s">
+        <v>173</v>
+      </c>
+      <c r="F29" s="106" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" s="33">
         <f>A28+1</f>
         <v>18</v>
@@ -3578,13 +3575,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C32" s="11">
         <v>6</v>
@@ -3599,96 +3596,96 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" hidden="1">
       <c r="A33" s="42">
         <f>A32+0.1</f>
         <v>19.100000000000001</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C33" s="41">
         <f>C32</f>
         <v>6</v>
       </c>
       <c r="D33" s="44" t="str">
-        <f t="shared" ref="D33:D38" si="14">D32</f>
+        <f t="shared" ref="D33:D38" si="15">D32</f>
         <v>Task</v>
       </c>
       <c r="E33" s="44" t="str">
-        <f t="shared" ref="E33:E38" si="15">E32</f>
+        <f t="shared" ref="E33:E38" si="16">E32</f>
         <v>Filter</v>
       </c>
       <c r="F33" s="45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" hidden="1">
       <c r="A34" s="42">
         <f>A33+0.1</f>
         <v>19.200000000000003</v>
       </c>
       <c r="B34" s="43" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C34" s="41">
-        <f>C32</f>
+        <f t="shared" ref="C34:E35" si="17">C32</f>
         <v>6</v>
       </c>
       <c r="D34" s="44" t="str">
-        <f>D32</f>
+        <f t="shared" si="17"/>
         <v>Task</v>
       </c>
       <c r="E34" s="44" t="str">
-        <f>E32</f>
+        <f t="shared" si="17"/>
         <v>Filter</v>
       </c>
       <c r="F34" s="45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" hidden="1">
       <c r="A35" s="42">
         <f>A34+0.1</f>
         <v>19.300000000000004</v>
       </c>
       <c r="B35" s="43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C35" s="41">
-        <f>C33</f>
+        <f t="shared" si="17"/>
         <v>6</v>
       </c>
       <c r="D35" s="44" t="str">
-        <f>D33</f>
+        <f t="shared" si="17"/>
         <v>Task</v>
       </c>
       <c r="E35" s="44" t="str">
-        <f>E33</f>
+        <f t="shared" si="17"/>
         <v>Filter</v>
       </c>
       <c r="F35" s="45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="42">
         <f>A35+0.1</f>
         <v>19.400000000000006</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C36" s="41">
-        <f t="shared" ref="C36" si="16">C35</f>
+        <f t="shared" ref="C36" si="18">C35</f>
         <v>6</v>
       </c>
       <c r="D36" s="44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Task</v>
       </c>
       <c r="E36" s="44" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Filter</v>
       </c>
       <c r="F36" s="45" t="s">
@@ -3722,18 +3719,18 @@
         <v>20.100000000000001</v>
       </c>
       <c r="B38" s="43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C38" s="41">
         <f>C37</f>
         <v>1</v>
       </c>
       <c r="D38" s="44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Task</v>
       </c>
       <c r="E38" s="44" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Add Task</v>
       </c>
       <c r="F38" s="45" t="s">
@@ -3746,18 +3743,18 @@
         <v>20.200000000000003</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C39" s="41">
-        <f t="shared" ref="C39:C40" si="17">C38</f>
+        <f t="shared" ref="C39:C40" si="19">C38</f>
         <v>1</v>
       </c>
       <c r="D39" s="44" t="str">
-        <f t="shared" ref="D39:D40" si="18">D38</f>
+        <f t="shared" ref="D39:D40" si="20">D38</f>
         <v>Task</v>
       </c>
       <c r="E39" s="44" t="str">
-        <f t="shared" ref="E39:E40" si="19">E38</f>
+        <f t="shared" ref="E39:E40" si="21">E38</f>
         <v>Add Task</v>
       </c>
       <c r="F39" s="46" t="str">
@@ -3771,18 +3768,18 @@
         <v>20.300000000000004</v>
       </c>
       <c r="B40" s="43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C40" s="41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="D40" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>Task</v>
       </c>
       <c r="E40" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>Add Task</v>
       </c>
       <c r="F40" s="46" t="str">
@@ -3796,18 +3793,18 @@
         <v>20.400000000000006</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C41" s="41">
-        <f t="shared" ref="C41" si="20">C40</f>
+        <f t="shared" ref="C41" si="22">C40</f>
         <v>1</v>
       </c>
       <c r="D41" s="44" t="str">
-        <f t="shared" ref="D41" si="21">D40</f>
+        <f t="shared" ref="D41" si="23">D40</f>
         <v>Task</v>
       </c>
       <c r="E41" s="44" t="str">
-        <f t="shared" ref="E41" si="22">E40</f>
+        <f t="shared" ref="E41" si="24">E40</f>
         <v>Add Task</v>
       </c>
       <c r="F41" s="46" t="str">
@@ -3815,7 +3812,7 @@
         <v>L</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" hidden="1">
       <c r="A42" s="34">
         <f>A37+1</f>
         <v>21</v>
@@ -3838,7 +3835,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -3863,25 +3860,25 @@
         <v>22.1</v>
       </c>
       <c r="B44" s="43" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C44" s="41">
         <f>C43</f>
         <v>1</v>
       </c>
       <c r="D44" s="44" t="str">
-        <f t="shared" ref="D44:E44" si="23">D43</f>
+        <f t="shared" ref="D44:E44" si="25">D43</f>
         <v>Task</v>
       </c>
       <c r="E44" s="44" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>Delete Task</v>
       </c>
       <c r="F44" s="45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" hidden="1">
       <c r="A45" s="34">
         <f>A43+1</f>
         <v>23</v>
@@ -3902,31 +3899,31 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1">
       <c r="A46" s="42">
         <f>A45+0.1</f>
         <v>23.1</v>
       </c>
       <c r="B46" s="43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C46" s="41">
-        <f t="shared" ref="C46" si="24">C45</f>
+        <f t="shared" ref="C46" si="26">C45</f>
         <v>5</v>
       </c>
       <c r="D46" s="44" t="str">
-        <f t="shared" ref="D46" si="25">D45</f>
+        <f t="shared" ref="D46" si="27">D45</f>
         <v>Task</v>
       </c>
       <c r="E46" s="44" t="str">
-        <f t="shared" ref="E46" si="26">E45</f>
+        <f t="shared" ref="E46" si="28">E45</f>
         <v>Modify Task</v>
       </c>
-      <c r="F46" s="79" t="s">
+      <c r="F46" s="76" t="s">
         <v>46</v>
       </c>
       <c r="G46" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -3950,41 +3947,40 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" hidden="1">
       <c r="A48" s="34">
         <f>A47+1</f>
         <v>25</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C48" s="11">
-        <v>1</v>
+        <v>138</v>
+      </c>
+      <c r="C48" s="116">
+        <v>15</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" hidden="1">
       <c r="A49" s="42">
         <f>A47+0.1</f>
         <v>24.1</v>
       </c>
       <c r="B49" s="43" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C49" s="41">
-        <f t="shared" ref="C49:D49" si="27">C48</f>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D49" s="44" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="D49" si="29">D48</f>
         <v>Task</v>
       </c>
       <c r="E49" s="44" t="str">
@@ -3997,20 +3993,20 @@
       </c>
       <c r="G49" s="28"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" hidden="1">
       <c r="A50" s="42">
         <f>A48+0.1</f>
         <v>25.1</v>
       </c>
       <c r="B50" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="C50" s="41">
-        <f t="shared" ref="C50" si="28">C49</f>
-        <v>1</v>
+        <v>140</v>
+      </c>
+      <c r="C50" s="114">
+        <f t="shared" ref="C50" si="30">C49</f>
+        <v>15</v>
       </c>
       <c r="D50" s="44" t="str">
-        <f t="shared" ref="D50" si="29">D49</f>
+        <f t="shared" ref="D50" si="31">D49</f>
         <v>Task</v>
       </c>
       <c r="E50" s="44" t="s">
@@ -4021,32 +4017,32 @@
       </c>
       <c r="G50" s="28"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" hidden="1">
       <c r="A51" s="42">
         <f>A49+0.1</f>
         <v>24.200000000000003</v>
       </c>
       <c r="B51" s="43" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C51" s="41">
         <v>15</v>
       </c>
       <c r="D51" s="44" t="str">
-        <f t="shared" ref="D51" si="30">D50</f>
+        <f t="shared" ref="D51" si="32">D50</f>
         <v>Task</v>
       </c>
       <c r="E51" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="F51" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="F51" s="76" t="s">
         <v>46</v>
       </c>
       <c r="G51" s="28" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" hidden="1">
       <c r="A52" s="34">
         <f>A47+1</f>
         <v>25</v>
@@ -4069,7 +4065,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -4088,9 +4084,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" hidden="1">
       <c r="A54" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -4111,7 +4107,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="B55" s="4" t="s">
@@ -4130,13 +4126,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" hidden="1">
       <c r="A56" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C56" s="11">
         <v>2</v>
@@ -4145,19 +4141,19 @@
         <v>27</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" hidden="1">
       <c r="A57" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C57" s="11">
         <v>2</v>
@@ -4166,19 +4162,19 @@
         <v>27</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" hidden="1">
       <c r="A58" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C58" s="11">
         <v>2</v>
@@ -4187,19 +4183,19 @@
         <v>27</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F58" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" hidden="1">
       <c r="A59" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C59" s="11">
         <v>4</v>
@@ -4214,13 +4210,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" hidden="1">
       <c r="A60" s="34">
-        <f t="shared" ref="A60" si="31">A59+1</f>
+        <f t="shared" ref="A60" si="33">A59+1</f>
         <v>33</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C60" s="11">
         <v>9</v>
@@ -4235,9 +4231,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" hidden="1">
       <c r="A61" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="B61" s="22" t="s">
@@ -4256,13 +4252,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" hidden="1">
       <c r="A62" s="36">
         <f>A56+1</f>
         <v>30</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C62" s="15">
         <v>8</v>
@@ -4277,13 +4273,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" hidden="1">
       <c r="A63" s="36">
         <f>A58+1</f>
         <v>32</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C63" s="15">
         <v>8</v>
@@ -4298,13 +4294,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" hidden="1">
       <c r="A64" s="36">
         <f>A61+1</f>
         <v>35</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C64" s="15">
         <v>8</v>
@@ -4319,9 +4315,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" hidden="1">
       <c r="A65" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="B65" s="14" t="s">
@@ -4341,32 +4337,32 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="72" customFormat="1">
-      <c r="A66" s="105">
+    <row r="66" spans="1:6" s="69" customFormat="1" hidden="1">
+      <c r="A66" s="101">
         <f>A65+0.1</f>
         <v>36.1</v>
       </c>
-      <c r="B66" s="104" t="s">
-        <v>166</v>
-      </c>
-      <c r="C66" s="103">
+      <c r="B66" s="100" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" s="99">
         <f>C65</f>
         <v>8</v>
       </c>
-      <c r="D66" s="103" t="str">
-        <f t="shared" ref="D66:F66" si="32">D65</f>
+      <c r="D66" s="99" t="str">
+        <f t="shared" ref="D66:F66" si="34">D65</f>
         <v>Notifications</v>
       </c>
-      <c r="E66" s="103" t="str">
-        <f t="shared" si="32"/>
+      <c r="E66" s="99" t="str">
+        <f t="shared" si="34"/>
         <v>Notifications</v>
       </c>
-      <c r="F66" s="63" t="str">
-        <f t="shared" si="32"/>
+      <c r="F66" s="61" t="str">
+        <f t="shared" si="34"/>
         <v>H</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" hidden="1">
       <c r="A67" s="37">
         <f>A65+1</f>
         <v>37</v>
@@ -4387,13 +4383,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" hidden="1">
       <c r="A68" s="47">
         <f>A67+1</f>
         <v>38</v>
       </c>
       <c r="B68" s="48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C68" s="49">
         <v>10</v>
@@ -4408,61 +4404,61 @@
         <v>45</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="72" customFormat="1">
-      <c r="A69" s="100">
+    <row r="69" spans="1:6" s="69" customFormat="1" hidden="1">
+      <c r="A69" s="96">
         <f>A68+0.1</f>
         <v>38.1</v>
       </c>
-      <c r="B69" s="99" t="s">
-        <v>146</v>
-      </c>
-      <c r="C69" s="97">
-        <f t="shared" ref="C69:E72" si="33">C68</f>
+      <c r="B69" s="95" t="s">
+        <v>144</v>
+      </c>
+      <c r="C69" s="93">
+        <f t="shared" ref="C69:E72" si="35">C68</f>
         <v>10</v>
       </c>
-      <c r="D69" s="96" t="str">
-        <f t="shared" si="33"/>
+      <c r="D69" s="92" t="str">
+        <f t="shared" si="35"/>
         <v>Dependencies</v>
       </c>
-      <c r="E69" s="96" t="str">
-        <f t="shared" si="33"/>
+      <c r="E69" s="92" t="str">
+        <f t="shared" si="35"/>
         <v>Dependencies</v>
       </c>
-      <c r="F69" s="98" t="s">
+      <c r="F69" s="94" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="72" customFormat="1">
-      <c r="A70" s="100">
+    <row r="70" spans="1:6" s="69" customFormat="1" hidden="1">
+      <c r="A70" s="96">
         <f>A69+0.1</f>
         <v>38.200000000000003</v>
       </c>
-      <c r="B70" s="99" t="s">
-        <v>144</v>
-      </c>
-      <c r="C70" s="97">
-        <f t="shared" si="33"/>
+      <c r="B70" s="95" t="s">
+        <v>142</v>
+      </c>
+      <c r="C70" s="93">
+        <f t="shared" si="35"/>
         <v>10</v>
       </c>
-      <c r="D70" s="96" t="str">
-        <f t="shared" si="33"/>
+      <c r="D70" s="92" t="str">
+        <f t="shared" si="35"/>
         <v>Dependencies</v>
       </c>
-      <c r="E70" s="96" t="str">
-        <f t="shared" si="33"/>
+      <c r="E70" s="92" t="str">
+        <f t="shared" si="35"/>
         <v>Dependencies</v>
       </c>
-      <c r="F70" s="98" t="s">
+      <c r="F70" s="94" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" hidden="1">
       <c r="A71" s="47">
         <f>A68+1</f>
         <v>39</v>
       </c>
       <c r="B71" s="48" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C71" s="49">
         <v>10</v>
@@ -4477,31 +4473,31 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="72" customFormat="1">
-      <c r="A72" s="100">
+    <row r="72" spans="1:6" s="69" customFormat="1" hidden="1">
+      <c r="A72" s="96">
         <f>A71+0.1</f>
         <v>39.1</v>
       </c>
-      <c r="B72" s="101" t="s">
-        <v>147</v>
-      </c>
-      <c r="C72" s="97">
-        <f t="shared" si="33"/>
+      <c r="B72" s="97" t="s">
+        <v>145</v>
+      </c>
+      <c r="C72" s="93">
+        <f t="shared" si="35"/>
         <v>10</v>
       </c>
-      <c r="D72" s="96" t="str">
-        <f t="shared" si="33"/>
+      <c r="D72" s="92" t="str">
+        <f t="shared" si="35"/>
         <v>Dependencies</v>
       </c>
-      <c r="E72" s="96" t="str">
-        <f t="shared" si="33"/>
+      <c r="E72" s="92" t="str">
+        <f t="shared" si="35"/>
         <v>Dependencies</v>
       </c>
-      <c r="F72" s="98" t="s">
+      <c r="F72" s="94" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" hidden="1">
       <c r="A73" s="38">
         <f>A71+1</f>
         <v>40</v>
@@ -4522,9 +4518,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" hidden="1">
       <c r="A74" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="B74" s="6" t="s">
@@ -4544,9 +4540,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" hidden="1">
       <c r="A75" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -4566,9 +4562,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" hidden="1">
       <c r="A76" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43</v>
       </c>
       <c r="B76" s="20" t="s">
@@ -4587,9 +4583,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" hidden="1">
       <c r="A77" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="B77" s="20" t="s">
@@ -4609,16 +4605,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" hidden="1">
       <c r="A78" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="B78" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C78" s="21">
-        <f t="shared" ref="C78:C84" si="34">C77</f>
+        <f t="shared" ref="C78:C84" si="36">C77</f>
         <v>12</v>
       </c>
       <c r="D78" s="20" t="s">
@@ -4631,16 +4627,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" hidden="1">
       <c r="A79" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>46</v>
       </c>
       <c r="B79" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C79" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>12</v>
       </c>
       <c r="D79" s="20" t="s">
@@ -4653,16 +4649,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" hidden="1">
       <c r="A80" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>47</v>
       </c>
       <c r="B80" s="20" t="s">
         <v>12</v>
       </c>
       <c r="C80" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>12</v>
       </c>
       <c r="D80" s="20" t="s">
@@ -4675,16 +4671,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" hidden="1">
       <c r="A81" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="B81" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C81" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>12</v>
       </c>
       <c r="D81" s="20" t="s">
@@ -4697,16 +4693,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" hidden="1">
       <c r="A82" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49</v>
       </c>
       <c r="B82" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C82" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>12</v>
       </c>
       <c r="D82" s="20" t="s">
@@ -4719,16 +4715,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" hidden="1">
       <c r="A83" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="B83" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C83" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>12</v>
       </c>
       <c r="D83" s="20" t="s">
@@ -4741,16 +4737,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" hidden="1">
       <c r="A84" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>51</v>
       </c>
       <c r="B84" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C84" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>12</v>
       </c>
       <c r="D84" s="20" t="s">
@@ -4763,216 +4759,222 @@
         <v>46</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
-      <c r="A85" s="81">
-        <f t="shared" si="4"/>
+    <row r="85" spans="1:7" hidden="1">
+      <c r="A85" s="78">
+        <f t="shared" si="5"/>
         <v>52</v>
       </c>
-      <c r="B85" s="61" t="s">
-        <v>100</v>
-      </c>
-      <c r="C85" s="82">
+      <c r="B85" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" s="79">
         <v>11</v>
       </c>
-      <c r="D85" s="61" t="s">
+      <c r="D85" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="E85" s="61" t="s">
+      <c r="E85" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="F85" s="83" t="s">
+      <c r="F85" s="80" t="s">
         <v>46</v>
       </c>
       <c r="G85" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" s="86">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" hidden="1">
+      <c r="A86" s="83">
         <f>A85+0.1</f>
         <v>52.1</v>
       </c>
-      <c r="B86" s="87" t="s">
-        <v>101</v>
-      </c>
-      <c r="C86" s="85">
-        <f t="shared" ref="C86:E88" si="35">C85</f>
+      <c r="B86" s="84" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" s="82">
+        <f t="shared" ref="C86:E88" si="37">C85</f>
         <v>11</v>
       </c>
-      <c r="D86" s="84" t="str">
-        <f t="shared" si="35"/>
+      <c r="D86" s="81" t="str">
+        <f t="shared" si="37"/>
         <v>Task</v>
       </c>
-      <c r="E86" s="84" t="str">
-        <f t="shared" si="35"/>
+      <c r="E86" s="81" t="str">
+        <f t="shared" si="37"/>
         <v>Modify Project</v>
       </c>
-      <c r="F86" s="88" t="s">
+      <c r="F86" s="85" t="s">
         <v>46</v>
       </c>
       <c r="G86" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" s="86">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" hidden="1">
+      <c r="A87" s="83">
         <f>A86+0.1</f>
         <v>52.2</v>
       </c>
-      <c r="B87" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="C87" s="85">
-        <f t="shared" si="35"/>
+      <c r="B87" s="84" t="s">
+        <v>100</v>
+      </c>
+      <c r="C87" s="82">
+        <f t="shared" si="37"/>
         <v>11</v>
       </c>
-      <c r="D87" s="84" t="s">
+      <c r="D87" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="E87" s="84" t="str">
-        <f t="shared" si="35"/>
+      <c r="E87" s="81" t="str">
+        <f t="shared" si="37"/>
         <v>Modify Project</v>
       </c>
-      <c r="F87" s="88" t="s">
+      <c r="F87" s="85" t="s">
         <v>46</v>
       </c>
       <c r="G87" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="86">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" hidden="1">
+      <c r="A88" s="83">
         <f>A87+0.1</f>
         <v>52.300000000000004</v>
       </c>
-      <c r="B88" s="87" t="s">
-        <v>103</v>
-      </c>
-      <c r="C88" s="85">
-        <f t="shared" si="35"/>
+      <c r="B88" s="84" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" s="82">
+        <f t="shared" si="37"/>
         <v>11</v>
       </c>
-      <c r="D88" s="84" t="str">
-        <f t="shared" si="35"/>
+      <c r="D88" s="81" t="str">
+        <f t="shared" si="37"/>
         <v>Project</v>
       </c>
-      <c r="E88" s="84" t="str">
-        <f t="shared" si="35"/>
+      <c r="E88" s="81" t="str">
+        <f t="shared" si="37"/>
         <v>Modify Project</v>
       </c>
-      <c r="F88" s="88" t="s">
+      <c r="F88" s="85" t="s">
         <v>46</v>
       </c>
       <c r="G88" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" s="106">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" hidden="1">
+      <c r="A89" s="102">
         <f>A85+1</f>
         <v>53</v>
       </c>
-      <c r="B89" s="107" t="s">
+      <c r="B89" s="103" t="s">
+        <v>168</v>
+      </c>
+      <c r="C89" s="104">
+        <v>16</v>
+      </c>
+      <c r="D89" s="103" t="s">
+        <v>169</v>
+      </c>
+      <c r="E89" s="103" t="s">
         <v>170</v>
       </c>
-      <c r="C89" s="108">
-        <v>16</v>
-      </c>
-      <c r="D89" s="107" t="s">
-        <v>171</v>
-      </c>
-      <c r="E89" s="107" t="s">
+      <c r="F89" s="105" t="s">
+        <v>46</v>
+      </c>
+      <c r="G89" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="91"/>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="119" t="s">
+        <v>120</v>
+      </c>
+      <c r="B93" s="119"/>
+      <c r="C93" s="119"/>
+      <c r="D93" s="119"/>
+      <c r="E93" s="119"/>
+      <c r="F93" s="119"/>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="B94" s="98" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="B95" s="98" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="B96" s="98" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="B97" s="98" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="B98" s="98" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="119" t="s">
         <v>172</v>
       </c>
-      <c r="F89" s="109" t="s">
-        <v>46</v>
-      </c>
-      <c r="G89" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92" s="95"/>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93" s="94" t="s">
-        <v>122</v>
-      </c>
-      <c r="B93" s="94"/>
-      <c r="C93" s="94"/>
-      <c r="D93" s="94"/>
-      <c r="E93" s="94"/>
-      <c r="F93" s="94"/>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="B94" s="102" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7">
-      <c r="B95" s="102" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="B96" s="102" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="B97" s="102" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="B98" s="102" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="94" t="s">
-        <v>174</v>
-      </c>
-      <c r="B101" s="94" t="s">
-        <v>174</v>
-      </c>
-      <c r="C101" s="94"/>
-      <c r="D101" s="94"/>
-      <c r="E101" s="94"/>
-      <c r="F101" s="94"/>
+      <c r="B101" s="119" t="s">
+        <v>172</v>
+      </c>
+      <c r="C101" s="119"/>
+      <c r="D101" s="119"/>
+      <c r="E101" s="119"/>
+      <c r="F101" s="119"/>
     </row>
     <row r="102" spans="1:6">
       <c r="B102" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="B103" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="B104" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="B105" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="B106" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="B107" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E84" xr:uid="{61C59655-00C9-AE4A-BEB6-766BC90BF29F}"/>
+  <autoFilter ref="A1:E89" xr:uid="{61C59655-00C9-AE4A-BEB6-766BC90BF29F}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="A93:F93"/>
     <mergeCell ref="A101:F101"/>
@@ -4986,10 +4988,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97AB1BC7-B588-5546-BFB9-55252DA1A1B6}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5007,279 +5009,300 @@
       <c r="C1" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="117" t="s">
+        <v>215</v>
+      </c>
+      <c r="K1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="52" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>94</v>
+        <v>76</v>
+      </c>
+      <c r="I2" s="74" t="s">
+        <v>216</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="52" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>86</v>
+        <v>220</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>216</v>
-      </c>
-      <c r="I3" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="I3" s="74" t="s">
+        <v>217</v>
+      </c>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E4" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="G4" s="115" t="s">
         <v>208</v>
       </c>
-      <c r="G4" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="I4" s="14"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="80" t="s">
-        <v>98</v>
+        <v>82</v>
+      </c>
+      <c r="F5" s="77" t="s">
+        <v>96</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="I5" s="63" t="s">
-        <v>70</v>
+        <v>207</v>
+      </c>
+      <c r="K5" s="61" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="14"/>
+        <v>78</v>
+      </c>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" s="116" t="s">
-        <v>181</v>
-      </c>
-      <c r="I7" s="14"/>
+        <v>90</v>
+      </c>
+      <c r="G7" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="52" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="H9" s="77" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:11">
+      <c r="A10" s="16" t="s">
+        <v>223</v>
+      </c>
       <c r="G10" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="G11" s="22" t="s">
-        <v>178</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="G12" s="22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="G13" s="22" t="s">
-        <v>99</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="G14" s="22" t="s">
-        <v>80</v>
+        <v>97</v>
+      </c>
+      <c r="H14" s="77" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="G15" s="22" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="B16" s="60" t="s">
+      <c r="G16" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="G17" s="118" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="B18" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="78" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="55" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="B17" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="77" t="s">
+      <c r="C18" s="75" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="75" t="s">
+        <v>218</v>
+      </c>
+      <c r="G18" s="55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="B19" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="74" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="B20" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="62" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="56" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="B18" s="48" t="s">
+      <c r="C20" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="77" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="56" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="C19" s="77" t="s">
+      <c r="E20" s="74" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="21">
-      <c r="A21" s="115" t="s">
+    <row r="21" spans="1:11">
+      <c r="C21" s="77" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="21">
+      <c r="A23" s="111" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="17" thickBot="1"/>
+    <row r="25" spans="1:11" s="86" customFormat="1" ht="32" customHeight="1" thickBot="1">
+      <c r="A25" s="108" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" s="108" t="s">
+        <v>185</v>
+      </c>
+      <c r="E25" s="108" t="s">
+        <v>187</v>
+      </c>
+      <c r="G25" s="108" t="s">
+        <v>191</v>
+      </c>
+      <c r="I25" s="108" t="s">
+        <v>196</v>
+      </c>
+      <c r="K25" s="108" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="110" customFormat="1" ht="102">
+      <c r="A26" s="109" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="109" t="s">
+        <v>186</v>
+      </c>
+      <c r="E26" s="109" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="17" thickBot="1"/>
-    <row r="23" spans="1:11" s="89" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A23" s="112" t="s">
-        <v>185</v>
-      </c>
-      <c r="C23" s="112" t="s">
-        <v>187</v>
-      </c>
-      <c r="E23" s="112" t="s">
+      <c r="G26" s="109" t="s">
+        <v>192</v>
+      </c>
+      <c r="I26" s="109" t="s">
+        <v>205</v>
+      </c>
+      <c r="K26" s="109" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="21">
+      <c r="A28" s="111" t="s">
         <v>189</v>
       </c>
-      <c r="G23" s="112" t="s">
+    </row>
+    <row r="29" spans="1:11" ht="17" thickBot="1"/>
+    <row r="30" spans="1:11" s="86" customFormat="1" ht="32" customHeight="1" thickBot="1">
+      <c r="A30" s="108" t="s">
         <v>193</v>
       </c>
-      <c r="I23" s="112" t="s">
+      <c r="C30" s="108" t="s">
+        <v>195</v>
+      </c>
+      <c r="E30" s="108" t="s">
         <v>198</v>
       </c>
-      <c r="K23" s="112" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="114" customFormat="1" ht="102">
-      <c r="A24" s="113" t="s">
+      <c r="G30" s="108"/>
+      <c r="I30" s="108"/>
+      <c r="K30" s="108"/>
+    </row>
+    <row r="31" spans="1:11" s="110" customFormat="1" ht="34">
+      <c r="A31" s="109" t="s">
+        <v>194</v>
+      </c>
+      <c r="C31" s="109" t="s">
         <v>186</v>
       </c>
-      <c r="C24" s="113" t="s">
-        <v>188</v>
-      </c>
-      <c r="E24" s="113" t="s">
-        <v>192</v>
-      </c>
-      <c r="G24" s="113" t="s">
-        <v>194</v>
-      </c>
-      <c r="I24" s="113" t="s">
-        <v>207</v>
-      </c>
-      <c r="K24" s="113" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="21">
-      <c r="A26" s="115" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="17" thickBot="1"/>
-    <row r="28" spans="1:11" s="89" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A28" s="112" t="s">
-        <v>195</v>
-      </c>
-      <c r="C28" s="112" t="s">
+      <c r="E31" s="109" t="s">
         <v>197</v>
       </c>
-      <c r="E28" s="112" t="s">
-        <v>200</v>
-      </c>
-      <c r="G28" s="112"/>
-      <c r="I28" s="112"/>
-      <c r="K28" s="112"/>
-    </row>
-    <row r="29" spans="1:11" s="114" customFormat="1" ht="34">
-      <c r="A29" s="113" t="s">
-        <v>196</v>
-      </c>
-      <c r="C29" s="113" t="s">
-        <v>188</v>
-      </c>
-      <c r="E29" s="113" t="s">
+      <c r="G31" s="109" t="s">
         <v>199</v>
       </c>
-      <c r="G29" s="113" t="s">
-        <v>201</v>
-      </c>
-      <c r="I29" s="113" t="s">
-        <v>201</v>
-      </c>
-      <c r="K29" s="113" t="s">
-        <v>201</v>
+      <c r="I31" s="109" t="s">
+        <v>199</v>
+      </c>
+      <c r="K31" s="109" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -5289,6 +5312,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42A419A-D42D-774B-89B4-9D99CC02BD75}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AAD82F-57B6-074F-8E66-CD602D7E6858}">
   <dimension ref="A1:A12"/>
   <sheetViews>
@@ -5298,52 +5336,50 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="117" t="s">
-        <v>212</v>
+      <c r="A1" s="113" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="111" t="s">
-        <v>213</v>
+      <c r="A2" s="107" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="111" t="s">
-        <v>214</v>
+      <c r="A3" s="107" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="111" t="s">
-        <v>215</v>
-      </c>
+      <c r="A4" s="107"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="111"/>
+      <c r="A5" s="107"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="111"/>
+      <c r="A6" s="107"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="111"/>
+      <c r="A7" s="107"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="111"/>
+      <c r="A8" s="107"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="111"/>
+      <c r="A9" s="107"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="111"/>
+      <c r="A10" s="107"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="111"/>
+      <c r="A11" s="107"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="111"/>
+      <c r="A12" s="107"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>